<commit_message>
changes on UI for box status and ui for closing the box
</commit_message>
<xml_diff>
--- a/docs/report.xlsx
+++ b/docs/report.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,77 +469,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>6818024906</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Lupin Pharmaceuticals, Inc.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>memantine hydrochloride</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>28 mg/1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>H102306</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>09/23/30</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>6330490190</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Sun Pharmaceutical Industries, Inc.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Fenofibrate</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>160 mg/1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MHC1672A</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>11/23/30</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4"/>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>